<commit_message>
First wave of updates from insittute PIs
</commit_message>
<xml_diff>
--- a/11-CollaborationList/LeoCancerCare.xlsx
+++ b/11-CollaborationList/LeoCancerCare.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11102"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ken.long/KL-GIT/CCAP/02-LhARA/00-Collaboration-lists/11-CollaborationList/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ken.long/Library/CloudStorage/Box-Box/CubMac-Box/KL-GIT/CCAP/02-LhARA/00-Collaboration-lists/11-CollaborationList/2025-11-Refresh/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{09A7289A-5018-4645-85D7-E671BC5F5CA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97BB0E1F-0A11-0D49-A0AE-C5D22A4379A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1100" yWindow="820" windowWidth="28040" windowHeight="17440" xr2:uid="{3B41F0D6-6DBE-EB4B-9E8B-E73C5290AB73}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="31">
   <si>
     <t>Title</t>
   </si>
@@ -94,19 +94,25 @@
     <t>Dr.</t>
   </si>
   <si>
-    <t>Patricia</t>
-  </si>
-  <si>
     <t>Underwood</t>
   </si>
   <si>
-    <t>P.</t>
-  </si>
-  <si>
     <t>tracy.underwood@leocancercare.com</t>
   </si>
   <si>
-    <t>P. Underwood</t>
+    <t>Tracy</t>
+  </si>
+  <si>
+    <t>T.</t>
+  </si>
+  <si>
+    <t>Bio-Med-UCL</t>
+  </si>
+  <si>
+    <t>Dept of Medical Physics and Biomedical Engineering, University College London, WC1E 6BT</t>
+  </si>
+  <si>
+    <t>T. Underwood</t>
   </si>
 </sst>
 </file>
@@ -993,8 +999,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8D64147-EF25-6F4C-A3A1-AF271DCEA121}">
   <dimension ref="A1:O3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:O3"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="N3" sqref="N3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1009,7 +1015,7 @@
     <col min="8" max="8" width="67.33203125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="21.83203125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="16.1640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="19" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="75.33203125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="17.1640625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="20" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="9.6640625" bestFit="1" customWidth="1"/>
@@ -1097,19 +1103,19 @@
         <v>23</v>
       </c>
       <c r="B3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" t="s">
         <v>24</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E3" t="s">
         <v>25</v>
       </c>
-      <c r="D3" t="s">
-        <v>26</v>
-      </c>
-      <c r="E3" t="s">
-        <v>27</v>
-      </c>
       <c r="F3" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="G3" t="s">
         <v>21</v>
@@ -1118,7 +1124,13 @@
         <v>22</v>
       </c>
       <c r="I3">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="J3" t="s">
+        <v>28</v>
+      </c>
+      <c r="K3" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>